<commit_message>
Risk Management Done, Needs checking
</commit_message>
<xml_diff>
--- a/Project Documents/IT_RiskAnalysisSheet.xlsx
+++ b/Project Documents/IT_RiskAnalysisSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael Chung\MITRE\MITR-RCC-Project\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D769D49-0234-47BE-8739-E9360AB5ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC6E078-17CE-4EC6-8AD8-BD1F42F0094D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>None</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Organizational Complexity</t>
   </si>
   <si>
-    <t>Percentage of business units affected</t>
-  </si>
-  <si>
     <t>Technology Risk</t>
   </si>
   <si>
@@ -60,27 +57,6 @@
     <t>Level of Customization required</t>
   </si>
   <si>
-    <t>Resource Risk</t>
-  </si>
-  <si>
-    <t>Availability of Resources</t>
-  </si>
-  <si>
-    <t>Skill level of Available Resources</t>
-  </si>
-  <si>
-    <t>Cost of training per personnel</t>
-  </si>
-  <si>
-    <t>Some</t>
-  </si>
-  <si>
-    <t>Almost All</t>
-  </si>
-  <si>
-    <t>Process Change Required</t>
-  </si>
-  <si>
     <t>Implementation Risk</t>
   </si>
   <si>
@@ -90,15 +66,6 @@
     <t>Configuration Detail required</t>
   </si>
   <si>
-    <t>All units</t>
-  </si>
-  <si>
-    <t>&gt; 50% units</t>
-  </si>
-  <si>
-    <t>&lt; 50% units</t>
-  </si>
-  <si>
     <t>0 - 3 months</t>
   </si>
   <si>
@@ -111,9 +78,6 @@
     <t>&gt; 24 months</t>
   </si>
   <si>
-    <t>Impact on Existing Systems</t>
-  </si>
-  <si>
     <t xml:space="preserve">Low </t>
   </si>
   <si>
@@ -123,9 +87,6 @@
     <t>Most/All</t>
   </si>
   <si>
-    <t xml:space="preserve">Medium </t>
-  </si>
-  <si>
     <t>Discount Rate</t>
   </si>
   <si>
@@ -157,17 +118,6 @@
   </si>
   <si>
     <t>Risk Index (0-100)</t>
-  </si>
-  <si>
-    <t>All 
-Available</t>
-  </si>
-  <si>
-    <t>None 
-Available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None  </t>
   </si>
   <si>
     <t>None units</t>
@@ -230,12 +180,39 @@
   <si>
     <t>Sum = 10</t>
   </si>
+  <si>
+    <t>Integration faults</t>
+  </si>
+  <si>
+    <t>Security Risk</t>
+  </si>
+  <si>
+    <t>Data Specificity</t>
+  </si>
+  <si>
+    <t>Cybersecurity threats</t>
+  </si>
+  <si>
+    <t>Regulatory compliance</t>
+  </si>
+  <si>
+    <t>Lack of User Acceptance</t>
+  </si>
+  <si>
+    <t>Change in Requirements</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>Medium amount</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -304,6 +281,18 @@
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -398,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -610,6 +599,8 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -931,7 +922,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -955,7 +946,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>3.3333333330000001</v>
@@ -970,16 +961,16 @@
     </row>
     <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E4" s="11">
         <v>3</v>
@@ -994,18 +985,18 @@
         <v>0</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="47">
         <v>0</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D5" s="19">
         <f>SUM(D6:D8)</f>
@@ -1027,7 +1018,7 @@
     </row>
     <row r="6" spans="1:9" ht="39" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="45">
         <v>1</v>
@@ -1046,18 +1037,18 @@
         <v>2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="39" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="45">
         <v>1</v>
@@ -1076,18 +1067,18 @@
         <v>2</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>0</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8" s="45">
         <v>0.6</v>
@@ -1106,13 +1097,13 @@
         <v>2</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -1128,17 +1119,17 @@
     </row>
     <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B10" s="47">
         <v>0</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D10" s="19">
-        <f>SUM(D11:D13)</f>
-        <v>20.333333331299997</v>
+        <f>SUM(D11:D12)</f>
+        <v>19.333333331399999</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>3</v>
@@ -1155,8 +1146,8 @@
       <c r="I10" s="28"/>
     </row>
     <row r="11" spans="1:9" ht="39" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>10</v>
+      <c r="A11" s="62" t="s">
+        <v>47</v>
       </c>
       <c r="B11" s="45">
         <v>1.9</v>
@@ -1169,24 +1160,24 @@
         <v>6.3333333326999997</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="39" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>48</v>
       </c>
       <c r="B12" s="45">
         <v>1.3</v>
@@ -1199,123 +1190,117 @@
         <v>12.9999999987</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="47">
+        <v>0</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="19">
+        <f>SUM(D15:D17)</f>
+        <v>4.9999999995</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="50">
         <v>1</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="39" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="45">
-        <v>0.3</v>
-      </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="21">
-        <f>C13*$B$3*B13</f>
-        <v>0.99999999989999999</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="47">
-        <v>0</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="19">
-        <f>SUM(D16:D17)</f>
-        <v>4.9999999995</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:9" ht="39" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="C16" s="50">
-        <v>1</v>
-      </c>
+      <c r="D15" s="21">
+        <f>C15*$B$3*B15</f>
+        <v>1.6666666665000001</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="48"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="21">
         <f>C16*$B$3*B16</f>
-        <v>1.6666666665000001</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>33</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:10" ht="39" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
-        <v>15</v>
+      <c r="A17" t="s">
+        <v>51</v>
       </c>
       <c r="B17" s="48">
         <v>0.5</v>
@@ -1328,19 +1313,19 @@
         <v>3.3333333330000001</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>0</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.25">
@@ -1356,13 +1341,13 @@
     </row>
     <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B19" s="47">
         <v>0</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D19" s="19">
         <f>SUM(D20:D21)</f>
@@ -1384,7 +1369,7 @@
     </row>
     <row r="20" spans="1:10" ht="39" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B20" s="48">
         <v>1.4</v>
@@ -1397,24 +1382,24 @@
         <v>4.6666666662000003</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="39" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B21" s="49">
         <v>1.5</v>
@@ -1433,13 +1418,13 @@
         <v>2</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H21" s="33" t="s">
         <v>0</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1456,15 +1441,15 @@
     </row>
     <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="18">
-        <f>SUM(D19,D15,D10,D5)</f>
-        <v>56.999999994299998</v>
+        <f>SUM(D19,D14,D10,D5)</f>
+        <v>55.9999999944</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
@@ -1487,12 +1472,12 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="61">
         <f>SUM(B5:B21)</f>
-        <v>10</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="B25" s="61"/>
       <c r="C25" s="39"/>
       <c r="D25" s="51" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1516,10 +1501,10 @@
       <c r="B27" s="54"/>
       <c r="C27" s="8"/>
       <c r="D27" s="52" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E27" s="53" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1531,7 +1516,7 @@
       <c r="B28" s="54"/>
       <c r="C28" s="8"/>
       <c r="D28" s="51" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E28" s="40">
         <v>0.5</v>
@@ -1546,7 +1531,7 @@
       <c r="B29" s="54"/>
       <c r="C29" s="8"/>
       <c r="D29" s="51" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E29" s="40">
         <v>0.4</v>
@@ -1561,7 +1546,7 @@
       <c r="B30" s="54"/>
       <c r="C30" s="8"/>
       <c r="D30" s="51" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E30" s="40">
         <v>0.3</v>
@@ -1576,7 +1561,7 @@
       <c r="B31" s="54"/>
       <c r="C31" s="8"/>
       <c r="D31" s="51" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E31" s="40">
         <v>0.2</v>
@@ -1591,7 +1576,7 @@
       <c r="B32" s="40"/>
       <c r="C32" s="40"/>
       <c r="D32" s="51" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E32" s="40">
         <v>0.16</v>
@@ -1606,7 +1591,7 @@
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
       <c r="D33" s="51" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E33" s="40">
         <v>0.14000000000000001</v>
@@ -1621,7 +1606,7 @@
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
       <c r="D34" s="51" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E34" s="40">
         <v>0.12</v>
@@ -1636,7 +1621,7 @@
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
       <c r="D35" s="51" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E35" s="40">
         <v>0.08</v>
@@ -1651,7 +1636,7 @@
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
       <c r="D36" s="57" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E36" s="40">
         <v>0.06</v>
@@ -1666,7 +1651,7 @@
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
       <c r="D37" s="57" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E37" s="40">
         <v>0.04</v>

</xml_diff>

<commit_message>
Changed time to organizational risk
</commit_message>
<xml_diff>
--- a/Project Documents/IT_RiskAnalysisSheet.xlsx
+++ b/Project Documents/IT_RiskAnalysisSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael Chung\MITRE\MITR-RCC-Project\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5ABD96-8C90-48B1-AB40-B7ECF7C694B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D31704C-44CB-477C-B7CC-BC6C76FB0569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <t>Categories in the website is not broad/specifc enough to encompass all CTF challenges.</t>
   </si>
   <si>
-    <t>The team is unable to provide the correct parameters/parameters are unable to be enforced</t>
+    <t>The team is unable to provide the correct tools to upload profiles and CTF challenges</t>
   </si>
 </sst>
 </file>
@@ -408,13 +408,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -516,10 +512,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -928,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -942,255 +934,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="62"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="27"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B3">
         <v>3.3333333330000001</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="27"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>3</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>1</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>0</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="45">
         <v>0</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <f>SUM(D6:D8)</f>
         <v>10.333333332300001</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="28"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="117" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="43">
         <v>0.5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <f>C6*$B$3*B6</f>
         <v>1.6666666665000001</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="104" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:9" ht="91" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="43">
         <v>0.2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <f>C7*$B$3*B7</f>
         <v>0.66666666660000007</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="43">
         <v>0.8</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>3</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <f>C8*$B$3*B8</f>
         <v>7.9999999991999999</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="28"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="45">
         <v>0</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <f>SUM(D11:D12)</f>
         <v>35.9999999964</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="28"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:9" ht="104" x14ac:dyDescent="0.3">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="43">
         <v>1.6</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>3</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <f>C11*$B$3*B11</f>
         <v>15.9999999984</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="28" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1198,128 +1190,128 @@
       <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="43">
         <v>2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>3</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <f>C12*$B$3*B12</f>
         <v>19.999999998</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="28" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="28"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="45">
         <v>0</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="19">
-        <f>SUM(D15:D17)</f>
-        <v>17.333333331600002</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="18">
+        <f>SUM(D15:D18)</f>
+        <v>18.999999998100002</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="65" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="46">
         <v>1.2</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="48">
         <v>2</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <f>C15*$B$3*B15</f>
         <v>7.9999999991999999</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="28" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="46">
         <v>0.8</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="48">
         <v>2</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <f>C16*$B$3*B16</f>
         <v>5.3333333328000005</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="28" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1327,433 +1319,422 @@
       <c r="A17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B17" s="46">
         <v>1.2</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <f>C17*$B$3*B17</f>
         <v>3.9999999996</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="28"/>
+    <row r="18" spans="1:10" ht="78" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="48">
+        <v>1</v>
+      </c>
+      <c r="D18" s="20">
+        <f>C18*$B$3*B18</f>
+        <v>1.6666666665000001</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="45">
         <v>0</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19">
-        <f>SUM(D20:D21)</f>
-        <v>9.6666666656999993</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="18">
+        <f>SUM(D21)</f>
+        <v>7.9999999991999999</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="28"/>
-    </row>
-    <row r="20" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="C20" s="50">
-        <v>1</v>
-      </c>
-      <c r="D20" s="21">
-        <f>C20*$B$3*B20</f>
-        <v>1.6666666665000001</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>53</v>
-      </c>
+      <c r="I19" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="91" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="47">
         <v>1.2</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>2</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <f>C21*$B$3*B21</f>
         <v>7.9999999991999999</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="18">
+      <c r="C23" s="22"/>
+      <c r="D23" s="17">
         <f>SUM(D19,D14,D10,D5)</f>
         <v>73.333333326000002</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="38"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="36"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="27"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="63">
+      <c r="A25" s="61">
         <f>SUM(B5:B21)</f>
         <v>9.9999999999999982</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="51" t="s">
+      <c r="B25" s="61"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="27"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="27"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="26"/>
     </row>
     <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="52" t="s">
+      <c r="A27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="27"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="51" t="s">
+      <c r="A28" s="52"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="40">
+      <c r="E28" s="38">
         <v>0.5</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="27"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="26"/>
     </row>
     <row r="29" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="51" t="s">
+      <c r="A29" s="52"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="40">
+      <c r="E29" s="38">
         <v>0.4</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="27"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="51" t="s">
+      <c r="A30" s="52"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="40">
+      <c r="E30" s="38">
         <v>0.3</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="27"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="51" t="s">
+      <c r="A31" s="52"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="38">
         <v>0.2</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="27"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="26"/>
     </row>
     <row r="32" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="51" t="s">
+      <c r="A32" s="52"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="38">
         <v>0.16</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="27"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="26"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="51" t="s">
+      <c r="A33" s="53"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="38">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="27"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="51" t="s">
+      <c r="A34" s="53"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="40">
+      <c r="E34" s="38">
         <v>0.12</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="27"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="51" t="s">
+      <c r="A35" s="54"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="40">
+      <c r="E35" s="38">
         <v>0.08</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="27"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="57" t="s">
+      <c r="A36" s="54"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="40">
+      <c r="E36" s="38">
         <v>0.06</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="27"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="57" t="s">
+      <c r="A37" s="54"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="40">
+      <c r="E37" s="38">
         <v>0.04</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="27"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="27"/>
+      <c r="A38" s="54"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="26"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="27"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="27"/>
+      <c r="A40" s="54"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="26"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="27"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="27"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="27"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>